<commit_message>
updated GH script and Psets and IFC models in new submission
</commit_message>
<xml_diff>
--- a/Psets.xlsx
+++ b/Psets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\2023\01\20230101\Delivery-Result\Codes\generic_anchors_ifc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA0A300A-BF6D-4DE3-A2B5-7D58D508F416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E556F5FA-031D-49DE-9B9C-4896A5A06530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3045" yWindow="1890" windowWidth="20040" windowHeight="15345" firstSheet="1" activeTab="7" xr2:uid="{D691B579-FABF-49B2-8F44-7CE73D92966A}"/>
+    <workbookView xWindow="18495" yWindow="1740" windowWidth="38595" windowHeight="18240" activeTab="1" xr2:uid="{D691B579-FABF-49B2-8F44-7CE73D92966A}"/>
   </bookViews>
   <sheets>
     <sheet name="A_MODELLINFO" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="113">
   <si>
     <t>parameter</t>
   </si>
@@ -165,12 +165,6 @@
     <t>Length</t>
   </si>
   <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Diameter</t>
-  </si>
-  <si>
     <t>[mm]</t>
   </si>
   <si>
@@ -186,202 +180,211 @@
     <t>Required type of head plate</t>
   </si>
   <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Azimuth</t>
+  </si>
+  <si>
+    <t>[°]</t>
+  </si>
+  <si>
+    <t>Inclination</t>
+  </si>
+  <si>
+    <t>Bond type</t>
+  </si>
+  <si>
+    <t>Bond length</t>
+  </si>
+  <si>
+    <t>Bond strength</t>
+  </si>
+  <si>
+    <t>Uniaxial Compressive Strength of bond material</t>
+  </si>
+  <si>
+    <t>[Pa]</t>
+  </si>
+  <si>
+    <t>Anchoring length</t>
+  </si>
+  <si>
+    <t>Inflation pressure</t>
+  </si>
+  <si>
+    <t>[bar]</t>
+  </si>
+  <si>
+    <t>Failure test recommended</t>
+  </si>
+  <si>
+    <t>Whether the failure test is recommended</t>
+  </si>
+  <si>
+    <t>Failure test</t>
+  </si>
+  <si>
+    <t>Whether the capacity of the installed anchor is tested against the yield load (Tested/Not tested)</t>
+  </si>
+  <si>
+    <t>Failure test force</t>
+  </si>
+  <si>
+    <t>Force that is applied in case it is yield load tested</t>
+  </si>
+  <si>
+    <t>Proof load test recommended</t>
+  </si>
+  <si>
+    <t>Whether the proof load test is recommended</t>
+  </si>
+  <si>
+    <t>Proof load test force</t>
+  </si>
+  <si>
+    <t>Force that is applied in case it is proof load tested</t>
+  </si>
+  <si>
+    <t>relevant</t>
+  </si>
+  <si>
+    <t>Combined Bolt</t>
+  </si>
+  <si>
+    <t>Cement</t>
+  </si>
+  <si>
+    <t>Circular</t>
+  </si>
+  <si>
+    <t>Proof load test</t>
+  </si>
+  <si>
+    <t>Required type of element</t>
+  </si>
+  <si>
+    <t>Unique identifier of single elements</t>
+  </si>
+  <si>
+    <t>Number of elements</t>
+  </si>
+  <si>
+    <t>Estimated number of elements in case no individual elements are modelled</t>
+  </si>
+  <si>
+    <t>Spacing of elements in case no individual elements are modelled</t>
+  </si>
+  <si>
+    <t>Estimated element length in case no individual elements are modelled, or specific lengths otherwise</t>
+  </si>
+  <si>
+    <t>Inclination from horizontal of individual element</t>
+  </si>
+  <si>
+    <t>Direction of individual element</t>
+  </si>
+  <si>
+    <t>Required yield load of element</t>
+  </si>
+  <si>
+    <t>Length of the element behind the zone subjected to displacement</t>
+  </si>
+  <si>
+    <t>Required pressure to inflate an expansion element (e.g. Swellex)</t>
+  </si>
+  <si>
+    <t>Material to be used to create an interface to the ground (e.g. cement, resin)</t>
+  </si>
+  <si>
+    <t>Length of the element that should be in contact with the ground</t>
+  </si>
+  <si>
+    <t>Pre-stressing force</t>
+  </si>
+  <si>
+    <t>Force that is to be applied in case of pre-stressed anchors</t>
+  </si>
+  <si>
+    <t>Element head X-coordinate</t>
+  </si>
+  <si>
+    <t>X-Coordinate of the element head</t>
+  </si>
+  <si>
+    <t>Element head Y-coordinate</t>
+  </si>
+  <si>
+    <t>Y-Coordinate of the element head</t>
+  </si>
+  <si>
+    <t>Element head Z-coordinate</t>
+  </si>
+  <si>
+    <t>Z-Coordinate of the element head</t>
+  </si>
+  <si>
+    <t>Measurement-while-drilling</t>
+  </si>
+  <si>
+    <t>Whether MWD data is available</t>
+  </si>
+  <si>
+    <t>Whether the capacity of the installed anchor is tested against the proof load and result (Passed/Failed/Not tested)</t>
+  </si>
+  <si>
+    <t>Current load</t>
+  </si>
+  <si>
+    <t>Current load determined by site testing/monitoring</t>
+  </si>
+  <si>
+    <t>Creep rate</t>
+  </si>
+  <si>
+    <t>Limit of the creep rate while testing</t>
+  </si>
+  <si>
+    <t>Slip</t>
+  </si>
+  <si>
+    <t>Slip while proof loading</t>
+  </si>
+  <si>
+    <t>Corrosion protection</t>
+  </si>
+  <si>
+    <t>Type of corrosion protection of the tensile element</t>
+  </si>
+  <si>
+    <t>Corrosion protection head</t>
+  </si>
+  <si>
+    <t>Type of corrosion protection of the head area</t>
+  </si>
+  <si>
+    <t>Element type</t>
+  </si>
+  <si>
+    <t>Reinforcement type (Active / Passive)</t>
+  </si>
+  <si>
+    <t>Element Diameter</t>
+  </si>
+  <si>
+    <t>Nominal diameter of rock bolts and anchors</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Whether the element is pre-stressed/active (Active) or non-stressed/passive (Passive)</t>
+  </si>
+  <si>
     <t>Active</t>
-  </si>
-  <si>
-    <t>Boolean</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Azimuth</t>
-  </si>
-  <si>
-    <t>[°]</t>
-  </si>
-  <si>
-    <t>Inclination</t>
-  </si>
-  <si>
-    <t>Bond type</t>
-  </si>
-  <si>
-    <t>Bond length</t>
-  </si>
-  <si>
-    <t>Bond strength</t>
-  </si>
-  <si>
-    <t>Uniaxial Compressive Strength of bond material</t>
-  </si>
-  <si>
-    <t>[Pa]</t>
-  </si>
-  <si>
-    <t>Anchoring length</t>
-  </si>
-  <si>
-    <t>Inflation pressure</t>
-  </si>
-  <si>
-    <t>[bar]</t>
-  </si>
-  <si>
-    <t>Failure test recommended</t>
-  </si>
-  <si>
-    <t>Whether the failure test is recommended</t>
-  </si>
-  <si>
-    <t>Failure test</t>
-  </si>
-  <si>
-    <t>Whether the capacity of the installed anchor is tested against the yield load (Tested/Not tested)</t>
-  </si>
-  <si>
-    <t>Failure test force</t>
-  </si>
-  <si>
-    <t>Force that is applied in case it is yield load tested</t>
-  </si>
-  <si>
-    <t>Proof load test recommended</t>
-  </si>
-  <si>
-    <t>Whether the proof load test is recommended</t>
-  </si>
-  <si>
-    <t>Proof load test force</t>
-  </si>
-  <si>
-    <t>Force that is applied in case it is proof load tested</t>
-  </si>
-  <si>
-    <t>relevant</t>
-  </si>
-  <si>
-    <t>Combined Bolt</t>
-  </si>
-  <si>
-    <t>Cement</t>
-  </si>
-  <si>
-    <t>Circular</t>
-  </si>
-  <si>
-    <t>Proof load test</t>
-  </si>
-  <si>
-    <t>Required type of element</t>
-  </si>
-  <si>
-    <t>Unique identifier of single elements</t>
-  </si>
-  <si>
-    <t>Whether the element is pre-stressed/active (True) or non-stressed/passive (False)</t>
-  </si>
-  <si>
-    <t>Number of elements</t>
-  </si>
-  <si>
-    <t>Estimated number of elements in case no individual elements are modelled</t>
-  </si>
-  <si>
-    <t>Spacing of elements in case no individual elements are modelled</t>
-  </si>
-  <si>
-    <t>Estimated element length in case no individual elements are modelled, or specific lengths otherwise</t>
-  </si>
-  <si>
-    <t>Inclination from horizontal of individual element</t>
-  </si>
-  <si>
-    <t>Direction of individual element</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nominal element diameter </t>
-  </si>
-  <si>
-    <t>Required yield load of element</t>
-  </si>
-  <si>
-    <t>Length of the element behind the zone subjected to displacement</t>
-  </si>
-  <si>
-    <t>Required pressure to inflate an expansion element (e.g. Swellex)</t>
-  </si>
-  <si>
-    <t>Material to be used to create an interface to the ground (e.g. cement, resin)</t>
-  </si>
-  <si>
-    <t>Length of the element that should be in contact with the ground</t>
-  </si>
-  <si>
-    <t>Pre-stressing force</t>
-  </si>
-  <si>
-    <t>Force that is to be applied in case of pre-stressed anchors</t>
-  </si>
-  <si>
-    <t>Element head X-coordinate</t>
-  </si>
-  <si>
-    <t>X-Coordinate of the element head</t>
-  </si>
-  <si>
-    <t>Element head Y-coordinate</t>
-  </si>
-  <si>
-    <t>Y-Coordinate of the element head</t>
-  </si>
-  <si>
-    <t>Element head Z-coordinate</t>
-  </si>
-  <si>
-    <t>Z-Coordinate of the element head</t>
-  </si>
-  <si>
-    <t>Measurement-while-drilling</t>
-  </si>
-  <si>
-    <t>Whether MWD data is available</t>
-  </si>
-  <si>
-    <t>Whether the capacity of the installed anchor is tested against the proof load and result (Passed/Failed/Not tested)</t>
-  </si>
-  <si>
-    <t>Current load</t>
-  </si>
-  <si>
-    <t>Current load determined by site testing/monitoring</t>
-  </si>
-  <si>
-    <t>Creep rate</t>
-  </si>
-  <si>
-    <t>Limit of the creep rate while testing</t>
-  </si>
-  <si>
-    <t>Slip</t>
-  </si>
-  <si>
-    <t>Slip while proof loading</t>
-  </si>
-  <si>
-    <t>Corrosion protection</t>
-  </si>
-  <si>
-    <t>Type of corrosion protection of the tensile element</t>
-  </si>
-  <si>
-    <t>Corrosion protection head</t>
-  </si>
-  <si>
-    <t>Type of corrosion protection of the head area</t>
-  </si>
-  <si>
-    <t>Passed</t>
   </si>
 </sst>
 </file>
@@ -972,8 +975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C9259D7-FEB3-418C-8720-A7065C1FE4BE}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1015,10 +1018,10 @@
     </row>
     <row r="2" spans="1:10" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>39</v>
+        <v>106</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>34</v>
@@ -1047,10 +1050,10 @@
     </row>
     <row r="3" spans="1:10" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>34</v>
@@ -1075,16 +1078,16 @@
     </row>
     <row r="4" spans="1:10" ht="132.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
-        <v>46</v>
+        <v>107</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>77</v>
+        <v>111</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>35</v>
@@ -1107,10 +1110,10 @@
     </row>
     <row r="5" spans="1:10" ht="96.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>34</v>
@@ -1132,7 +1135,7 @@
         <v>36</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>37</v>
@@ -1154,7 +1157,7 @@
         <v>38</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>37</v>
@@ -1181,13 +1184,13 @@
     </row>
     <row r="8" spans="1:10" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>21</v>
@@ -1209,13 +1212,13 @@
     </row>
     <row r="9" spans="1:10" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>21</v>
@@ -1235,15 +1238,15 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="80.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
-        <v>40</v>
+        <v>108</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>84</v>
+        <v>109</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>21</v>
@@ -1267,13 +1270,13 @@
     </row>
     <row r="11" spans="1:10" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>21</v>
@@ -1297,10 +1300,10 @@
     </row>
     <row r="12" spans="1:10" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>34</v>
@@ -1321,10 +1324,10 @@
     </row>
     <row r="13" spans="1:10" ht="108.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>37</v>
@@ -1349,13 +1352,13 @@
     </row>
     <row r="14" spans="1:10" ht="96.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>21</v>
@@ -1373,10 +1376,10 @@
     </row>
     <row r="15" spans="1:10" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>34</v>
@@ -1403,10 +1406,10 @@
     </row>
     <row r="16" spans="1:10" ht="96.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>37</v>
@@ -1433,13 +1436,13 @@
     </row>
     <row r="17" spans="1:10" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D17" s="12" t="s">
         <v>21</v>
@@ -1463,13 +1466,13 @@
     </row>
     <row r="18" spans="1:10" ht="84.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D18" s="12" t="s">
         <v>21</v>
@@ -1491,10 +1494,10 @@
     </row>
     <row r="19" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>34</v>
@@ -1519,10 +1522,10 @@
     </row>
     <row r="20" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C20" s="12" t="s">
         <v>34</v>
@@ -1547,10 +1550,10 @@
     </row>
     <row r="21" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>34</v>
@@ -1575,16 +1578,16 @@
     </row>
     <row r="22" spans="1:10" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C22" s="12" t="s">
         <v>34</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
@@ -1597,16 +1600,16 @@
     </row>
     <row r="23" spans="1:10" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>34</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E23" s="12"/>
       <c r="F23" s="12"/>
@@ -1621,16 +1624,16 @@
     </row>
     <row r="24" spans="1:10" ht="144.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C24" s="12" t="s">
         <v>34</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
@@ -1643,13 +1646,13 @@
     </row>
     <row r="25" spans="1:10" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D25" s="12" t="s">
         <v>21</v>
@@ -1665,16 +1668,16 @@
     </row>
     <row r="26" spans="1:10" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C26" s="12" t="s">
         <v>34</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E26" s="12"/>
       <c r="F26" s="12"/>
@@ -1689,10 +1692,10 @@
     </row>
     <row r="27" spans="1:10" ht="168.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C27" s="12" t="s">
         <v>34</v>
@@ -1711,13 +1714,13 @@
     </row>
     <row r="28" spans="1:10" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D28" s="12" t="s">
         <v>21</v>
@@ -1733,13 +1736,13 @@
     </row>
     <row r="29" spans="1:10" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D29" s="12" t="s">
         <v>21</v>
@@ -1755,13 +1758,13 @@
     </row>
     <row r="30" spans="1:10" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D30" s="12" t="s">
         <v>21</v>
@@ -1777,13 +1780,13 @@
     </row>
     <row r="31" spans="1:10" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D31" s="12" t="s">
         <v>21</v>
@@ -1799,10 +1802,10 @@
     </row>
     <row r="32" spans="1:10" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C32" s="12" t="s">
         <v>34</v>
@@ -1823,10 +1826,10 @@
     </row>
     <row r="33" spans="1:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C33" s="12" t="s">
         <v>34</v>
@@ -1856,7 +1859,7 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1877,20 +1880,20 @@
         <v>1</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="str">
         <f>'LOD-all'!A2</f>
-        <v>Type</v>
+        <v>Element type</v>
       </c>
       <c r="B2" s="6" t="str">
         <f>'LOD-all'!D2</f>
         <v>Text</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D2" s="6" t="str">
         <f>'LOD-all'!E2</f>
@@ -1915,14 +1918,14 @@
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="str">
         <f>'LOD-all'!A4</f>
-        <v>Active</v>
+        <v>Reinforcement type (Active / Passive)</v>
       </c>
       <c r="B4" s="6" t="str">
         <f>'LOD-all'!D4</f>
-        <v>Boolean</v>
-      </c>
-      <c r="C4" s="6" t="b">
-        <v>1</v>
+        <v>Text</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>112</v>
       </c>
       <c r="D4" s="6" t="str">
         <f>'LOD-all'!E4</f>
@@ -2007,7 +2010,7 @@
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="str">
         <f>'LOD-all'!A10</f>
-        <v>Diameter</v>
+        <v>Element Diameter</v>
       </c>
       <c r="B10" s="6" t="str">
         <f>'LOD-all'!D10</f>
@@ -2221,7 +2224,7 @@
       </c>
       <c r="B24" s="6" t="str">
         <f>'LOD-all'!D24</f>
-        <v>Boolean</v>
+        <v>Text</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="6">
@@ -2374,7 +2377,7 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C17"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2395,20 +2398,20 @@
         <v>1</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="str">
         <f>'LOD-all'!A2</f>
-        <v>Type</v>
+        <v>Element type</v>
       </c>
       <c r="B2" s="6" t="str">
         <f>'LOD-all'!D2</f>
         <v>Text</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D2" s="6" t="str">
         <f>'LOD-all'!F2</f>
@@ -2433,14 +2436,14 @@
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="str">
         <f>'LOD-all'!A4</f>
-        <v>Active</v>
+        <v>Reinforcement type (Active / Passive)</v>
       </c>
       <c r="B4" s="6" t="str">
         <f>'LOD-all'!D4</f>
-        <v>Boolean</v>
-      </c>
-      <c r="C4" s="6" t="b">
-        <v>1</v>
+        <v>Text</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>112</v>
       </c>
       <c r="D4" s="6" t="str">
         <f>'LOD-all'!F4</f>
@@ -2531,7 +2534,7 @@
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="str">
         <f>'LOD-all'!A10</f>
-        <v>Diameter</v>
+        <v>Element Diameter</v>
       </c>
       <c r="B10" s="6" t="str">
         <f>'LOD-all'!D10</f>
@@ -2617,7 +2620,7 @@
         <v>Text</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D15" s="6" t="str">
         <f>'LOD-all'!F15</f>
@@ -2755,7 +2758,7 @@
       </c>
       <c r="B24" s="6" t="str">
         <f>'LOD-all'!D24</f>
-        <v>Boolean</v>
+        <v>Text</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="6">
@@ -2908,7 +2911,7 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2928,20 +2931,20 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>'LOD-all'!A2</f>
-        <v>Type</v>
+        <v>Element type</v>
       </c>
       <c r="B2" t="str">
         <f>'LOD-all'!D2</f>
         <v>Text</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D2" t="str">
         <f>'LOD-all'!G2</f>
@@ -2966,14 +2969,14 @@
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>'LOD-all'!A4</f>
-        <v>Active</v>
+        <v>Reinforcement type (Active / Passive)</v>
       </c>
       <c r="B4" t="str">
         <f>'LOD-all'!D4</f>
-        <v>Boolean</v>
-      </c>
-      <c r="C4" s="6" t="b">
-        <v>1</v>
+        <v>Text</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>112</v>
       </c>
       <c r="D4" t="str">
         <f>'LOD-all'!G4</f>
@@ -2989,9 +2992,7 @@
         <f>'LOD-all'!D5</f>
         <v>Integer</v>
       </c>
-      <c r="C5" s="6">
-        <v>20</v>
-      </c>
+      <c r="C5" s="6"/>
       <c r="D5">
         <f>'LOD-all'!G5</f>
         <v>0</v>
@@ -3006,9 +3007,7 @@
         <f>'LOD-all'!D6</f>
         <v>Real</v>
       </c>
-      <c r="C6" s="6">
-        <v>2</v>
-      </c>
+      <c r="C6" s="6"/>
       <c r="D6">
         <f>'LOD-all'!G6</f>
         <v>0</v>
@@ -3064,7 +3063,7 @@
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>'LOD-all'!A10</f>
-        <v>Diameter</v>
+        <v>Element Diameter</v>
       </c>
       <c r="B10" t="str">
         <f>'LOD-all'!D10</f>
@@ -3152,7 +3151,7 @@
         <v>Text</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D15" t="str">
         <f>'LOD-all'!G15</f>
@@ -3292,7 +3291,7 @@
       </c>
       <c r="B24" t="str">
         <f>'LOD-all'!D24</f>
-        <v>Boolean</v>
+        <v>Text</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24">
@@ -3445,7 +3444,7 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C33"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3465,20 +3464,20 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>'LOD-all'!A2</f>
-        <v>Type</v>
+        <v>Element type</v>
       </c>
       <c r="B2" t="str">
         <f>'LOD-all'!D2</f>
         <v>Text</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D2" t="str">
         <f>'LOD-all'!H2</f>
@@ -3503,14 +3502,14 @@
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>'LOD-all'!A4</f>
-        <v>Active</v>
+        <v>Reinforcement type (Active / Passive)</v>
       </c>
       <c r="B4" t="str">
         <f>'LOD-all'!D4</f>
-        <v>Boolean</v>
-      </c>
-      <c r="C4" s="6" t="b">
-        <v>1</v>
+        <v>Text</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>112</v>
       </c>
       <c r="D4" t="str">
         <f>'LOD-all'!H4</f>
@@ -3526,9 +3525,7 @@
         <f>'LOD-all'!D5</f>
         <v>Integer</v>
       </c>
-      <c r="C5" s="6">
-        <v>20</v>
-      </c>
+      <c r="C5" s="6"/>
       <c r="D5">
         <f>'LOD-all'!H5</f>
         <v>0</v>
@@ -3543,9 +3540,7 @@
         <f>'LOD-all'!D6</f>
         <v>Real</v>
       </c>
-      <c r="C6" s="6">
-        <v>2</v>
-      </c>
+      <c r="C6" s="6"/>
       <c r="D6">
         <f>'LOD-all'!H6</f>
         <v>0</v>
@@ -3601,7 +3596,7 @@
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>'LOD-all'!A10</f>
-        <v>Diameter</v>
+        <v>Element Diameter</v>
       </c>
       <c r="B10" t="str">
         <f>'LOD-all'!D10</f>
@@ -3689,7 +3684,7 @@
         <v>Text</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D15" t="str">
         <f>'LOD-all'!H15</f>
@@ -3829,7 +3824,7 @@
       </c>
       <c r="B24" t="str">
         <f>'LOD-all'!D24</f>
-        <v>Boolean</v>
+        <v>Text</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24">
@@ -3982,7 +3977,7 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4003,20 +3998,20 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>'LOD-all'!A2</f>
-        <v>Type</v>
+        <v>Element type</v>
       </c>
       <c r="B2" t="str">
         <f>'LOD-all'!D2</f>
         <v>Text</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D2" t="str">
         <f>'LOD-all'!I2</f>
@@ -4041,14 +4036,14 @@
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>'LOD-all'!A4</f>
-        <v>Active</v>
+        <v>Reinforcement type (Active / Passive)</v>
       </c>
       <c r="B4" t="str">
         <f>'LOD-all'!D4</f>
-        <v>Boolean</v>
-      </c>
-      <c r="C4" s="6" t="b">
-        <v>1</v>
+        <v>Text</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>112</v>
       </c>
       <c r="D4" t="str">
         <f>'LOD-all'!I4</f>
@@ -4064,9 +4059,7 @@
         <f>'LOD-all'!D5</f>
         <v>Integer</v>
       </c>
-      <c r="C5" s="6">
-        <v>20</v>
-      </c>
+      <c r="C5" s="6"/>
       <c r="D5">
         <f>'LOD-all'!I5</f>
         <v>0</v>
@@ -4081,9 +4074,7 @@
         <f>'LOD-all'!D6</f>
         <v>Real</v>
       </c>
-      <c r="C6" s="6">
-        <v>2</v>
-      </c>
+      <c r="C6" s="6"/>
       <c r="D6">
         <f>'LOD-all'!I6</f>
         <v>0</v>
@@ -4139,7 +4130,7 @@
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>'LOD-all'!A10</f>
-        <v>Diameter</v>
+        <v>Element Diameter</v>
       </c>
       <c r="B10" t="str">
         <f>'LOD-all'!D10</f>
@@ -4180,7 +4171,7 @@
         <v>Text</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D12" t="str">
         <f>'LOD-all'!I12</f>
@@ -4231,7 +4222,7 @@
         <v>Text</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D15" t="str">
         <f>'LOD-all'!I15</f>
@@ -4371,7 +4362,7 @@
       </c>
       <c r="B24" t="str">
         <f>'LOD-all'!D24</f>
-        <v>Boolean</v>
+        <v>Text</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24">
@@ -4523,8 +4514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFE1EA75-E0E7-4DF4-8845-DC25E0A1284C}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J27" sqref="J26:J27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4545,20 +4536,20 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>'LOD-all'!A2</f>
-        <v>Type</v>
+        <v>Element type</v>
       </c>
       <c r="B2" t="str">
         <f>'LOD-all'!D2</f>
         <v>Text</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D2" t="str">
         <f>'LOD-all'!J2</f>
@@ -4583,14 +4574,14 @@
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>'LOD-all'!A4</f>
-        <v>Active</v>
+        <v>Reinforcement type (Active / Passive)</v>
       </c>
       <c r="B4" t="str">
         <f>'LOD-all'!D4</f>
-        <v>Boolean</v>
-      </c>
-      <c r="C4" s="6" t="b">
-        <v>1</v>
+        <v>Text</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>112</v>
       </c>
       <c r="D4" t="str">
         <f>'LOD-all'!J4</f>
@@ -4606,9 +4597,7 @@
         <f>'LOD-all'!D5</f>
         <v>Integer</v>
       </c>
-      <c r="C5" s="6">
-        <v>20</v>
-      </c>
+      <c r="C5" s="6"/>
       <c r="D5">
         <f>'LOD-all'!J5</f>
         <v>0</v>
@@ -4623,9 +4612,7 @@
         <f>'LOD-all'!D6</f>
         <v>Real</v>
       </c>
-      <c r="C6" s="6">
-        <v>2</v>
-      </c>
+      <c r="C6" s="6"/>
       <c r="D6">
         <f>'LOD-all'!J6</f>
         <v>0</v>
@@ -4681,7 +4668,7 @@
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>'LOD-all'!A10</f>
-        <v>Diameter</v>
+        <v>Element Diameter</v>
       </c>
       <c r="B10" t="str">
         <f>'LOD-all'!D10</f>
@@ -4722,7 +4709,7 @@
         <v>Text</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D12" t="str">
         <f>'LOD-all'!J12</f>
@@ -4773,7 +4760,7 @@
         <v>Text</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D15" t="str">
         <f>'LOD-all'!J15</f>
@@ -4885,7 +4872,9 @@
         <f>'LOD-all'!D22</f>
         <v>Boolean</v>
       </c>
-      <c r="C22" s="6"/>
+      <c r="C22" s="6" t="s">
+        <v>110</v>
+      </c>
       <c r="D22" t="str">
         <f>'LOD-all'!J22</f>
         <v>X</v>
@@ -4913,7 +4902,7 @@
       </c>
       <c r="B24" t="str">
         <f>'LOD-all'!D24</f>
-        <v>Boolean</v>
+        <v>Text</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" t="str">
@@ -4930,9 +4919,7 @@
         <f>'LOD-all'!D25</f>
         <v>Real</v>
       </c>
-      <c r="C25" s="6">
-        <v>402</v>
-      </c>
+      <c r="C25" s="6"/>
       <c r="D25" t="str">
         <f>'LOD-all'!J25</f>
         <v>X</v>
@@ -4962,9 +4949,7 @@
         <f>'LOD-all'!D27</f>
         <v>Text</v>
       </c>
-      <c r="C27" s="6" t="s">
-        <v>111</v>
-      </c>
+      <c r="C27" s="6"/>
       <c r="D27" t="str">
         <f>'LOD-all'!J27</f>
         <v>X</v>
@@ -4979,9 +4964,7 @@
         <f>'LOD-all'!D28</f>
         <v>Real</v>
       </c>
-      <c r="C28" s="6">
-        <v>160</v>
-      </c>
+      <c r="C28" s="6"/>
       <c r="D28" t="str">
         <f>'LOD-all'!J28</f>
         <v>X</v>

</xml_diff>